<commit_message>
Added Frontend services for orders and implemented pdf for menus
</commit_message>
<xml_diff>
--- a/Doku/zeitplan_HungerSatt.xlsx
+++ b/Doku/zeitplan_HungerSatt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlsaalfelden322-my.sharepoint.com/personal/johannes_ellmer_htl-saalfelden_at/Documents/Dokumente/GitHub/Diplomarbeit_Bestellapp/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{3460CF72-AC89-4CED-8824-3C5C9549F2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67ABFDA9-3A14-48AD-B30D-FDE88596E3C6}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{3460CF72-AC89-4CED-8824-3C5C9549F2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08F4E60-AAE5-49AB-B84A-C81A912A30C3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="735" yWindow="735" windowWidth="18000" windowHeight="10433" xr2:uid="{72F4632B-4B3C-4A8B-9C92-C659B892C97E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{72F4632B-4B3C-4A8B-9C92-C659B892C97E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <t>Hosting des Frontend</t>
   </si>
   <si>
-    <t>Proxmox Server aufsetzen und einrichten</t>
+    <t>Hosting Planen</t>
   </si>
 </sst>
 </file>
@@ -643,15 +643,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -685,53 +732,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:AI51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1183,65 +1183,65 @@
       <c r="AD19" s="9"/>
     </row>
     <row r="20" spans="1:34" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="49" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="49" t="s">
+      <c r="E20" s="67"/>
+      <c r="F20" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42" t="s">
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42" t="s">
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42" t="s">
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
-      <c r="U20" s="42"/>
-      <c r="V20" s="42" t="s">
+      <c r="S20" s="59"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+      <c r="V20" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="W20" s="42"/>
-      <c r="X20" s="42"/>
-      <c r="Y20" s="42"/>
-      <c r="Z20" s="42" t="s">
+      <c r="W20" s="59"/>
+      <c r="X20" s="59"/>
+      <c r="Y20" s="59"/>
+      <c r="Z20" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="AA20" s="42"/>
-      <c r="AB20" s="42"/>
-      <c r="AC20" s="42"/>
-      <c r="AD20" s="43"/>
-      <c r="AE20" s="37" t="s">
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="59"/>
+      <c r="AC20" s="59"/>
+      <c r="AD20" s="60"/>
+      <c r="AE20" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="38"/>
+      <c r="AF20" s="55"/>
+      <c r="AG20" s="55"/>
+      <c r="AH20" s="56"/>
     </row>
     <row r="21" spans="1:34" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="22" t="s">
         <v>3</v>
       </c>
@@ -1337,11 +1337,11 @@
       </c>
     </row>
     <row r="22" spans="1:34" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="7">
         <v>2</v>
       </c>
@@ -1353,11 +1353,11 @@
       <c r="AH22" s="8"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="7">
         <v>10</v>
       </c>
@@ -1370,11 +1370,11 @@
       <c r="AH23" s="8"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="7">
         <v>5</v>
       </c>
@@ -1385,11 +1385,11 @@
       <c r="AH24" s="8"/>
     </row>
     <row r="25" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="15">
         <f>SUM(D22:D24)</f>
         <v>17</v>
@@ -1440,17 +1440,19 @@
       <c r="E26" s="8">
         <v>10</v>
       </c>
-      <c r="I26" s="66"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="67"/>
+      <c r="I26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
       <c r="AH26" s="8"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="4">
         <f>SUM(D28:D33)</f>
         <v>41</v>
@@ -1463,11 +1465,11 @@
       <c r="AH27" s="8"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="53"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="45"/>
       <c r="D28">
         <v>9</v>
       </c>
@@ -1483,11 +1485,11 @@
       <c r="AH28" s="8"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="7">
         <v>8</v>
       </c>
@@ -1498,11 +1500,11 @@
       <c r="AH29" s="8"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="53"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
       <c r="D30">
         <v>10</v>
       </c>
@@ -1514,11 +1516,11 @@
       <c r="AH30" s="8"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="7">
         <v>10</v>
       </c>
@@ -1526,26 +1528,26 @@
         <v>2</v>
       </c>
       <c r="I31" s="29"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
       <c r="AH31" s="8"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="7">
         <v>0</v>
       </c>
       <c r="E32" s="8">
         <v>25</v>
       </c>
-      <c r="J32" s="66"/>
+      <c r="J32" s="37"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
       <c r="AH32" s="8"/>
     </row>
     <row r="33" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1591,11 +1593,11 @@
       <c r="AH33" s="10"/>
     </row>
     <row r="34" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="4">
         <f>SUM(D35:D39)</f>
         <v>30</v>
@@ -1608,77 +1610,77 @@
       <c r="AH34" s="8"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="7">
         <v>0</v>
       </c>
       <c r="E35" s="8">
         <v>10</v>
       </c>
-      <c r="N35" s="5"/>
+      <c r="N35" s="29"/>
       <c r="O35" s="5"/>
       <c r="AH35" s="8"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="53"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" s="8">
         <v>15</v>
       </c>
-      <c r="O36" s="5"/>
+      <c r="O36" s="29"/>
       <c r="P36" s="5"/>
       <c r="AH36" s="8"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="53"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="45"/>
       <c r="D37">
         <v>15</v>
       </c>
       <c r="E37" s="8">
         <v>5</v>
       </c>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
       <c r="P37" s="5"/>
       <c r="AH37" s="8"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="53"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="45"/>
       <c r="D38">
         <v>10</v>
       </c>
       <c r="E38" s="8">
         <v>1</v>
       </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
       <c r="AH38" s="8"/>
     </row>
     <row r="39" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="53"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="45"/>
       <c r="D39">
         <v>5</v>
       </c>
@@ -1692,11 +1694,11 @@
       <c r="AH39" s="10"/>
     </row>
     <row r="40" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="61"/>
-      <c r="C40" s="62"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="18">
         <f>SUM(D41:D43)</f>
         <v>38</v>
@@ -1780,11 +1782,11 @@
       <c r="AI43" s="7"/>
     </row>
     <row r="44" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="63" t="s">
+      <c r="A44" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="18">
         <f>SUM(D45:D46)</f>
         <v>15</v>
@@ -1833,6 +1835,7 @@
       </c>
       <c r="F45" s="7"/>
       <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
       <c r="AH45" s="8"/>
     </row>
     <row r="46" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1878,11 +1881,11 @@
       <c r="AH46" s="10"/>
     </row>
     <row r="47" spans="1:35" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="56"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="4">
         <v>60</v>
       </c>
@@ -1893,11 +1896,11 @@
       <c r="AH47" s="8"/>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="53"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="45"/>
       <c r="D48">
         <v>18</v>
       </c>
@@ -1922,8 +1925,10 @@
       <c r="E49" s="34">
         <v>40</v>
       </c>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
       <c r="V49" s="5"/>
       <c r="AB49" s="5"/>
       <c r="AC49" s="5"/>
@@ -1931,11 +1936,11 @@
       <c r="AH49" s="8"/>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="59"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="43"/>
       <c r="D50" s="35">
         <f>D25+D26+D27+D34+D40+D44+D47</f>
         <v>211</v>
@@ -1980,24 +1985,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
     <mergeCell ref="AE20:AH20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A23:C23"/>
@@ -2012,6 +1999,24 @@
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:M20"/>
     <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>